<commit_message>
Agregada la función de exportar padrón almacenado en la Base de Datos y pequeños cambios al procesamiento de lecturas desde los archivos de texto plano
</commit_message>
<xml_diff>
--- a/recursos/PADRON DE CLIENTES MAYORES MAYO ELS - Copy.xlsx
+++ b/recursos/PADRON DE CLIENTES MAYORES MAYO ELS - Copy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmorales\Desktop\PERFILES 2018\2019\MAYO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\OneDrive\Documentos\Repositorios\Lecuras-Medidor_2\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="TACNA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="LIBRES" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MOQUEGUA!$A$1:$EQ$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MOQUEGUA!$A$1:$EN$94</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TACNA!$A$1:$ET$580</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -4527,10 +4527,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -5053,7 +5053,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5072,9 +5072,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5085,9 +5085,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5103,6 +5100,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -5429,7 +5429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P580"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
@@ -34466,8 +34466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34481,11 +34481,11 @@
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -34521,19 +34521,19 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>14</v>
@@ -34570,20 +34570,20 @@
       <c r="J2" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="M2" s="3">
+        <v>38.181800000000003</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M2" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="O2" s="3">
-        <v>38.181800000000003</v>
       </c>
       <c r="P2" s="3">
         <v>1271989</v>
@@ -34620,20 +34620,20 @@
       <c r="J3" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M3" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P3" s="3">
         <v>2812212</v>
@@ -34670,20 +34670,20 @@
       <c r="J4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>20.818200000000001</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M4" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O4" s="3">
-        <v>20.818200000000001</v>
       </c>
       <c r="P4" s="3">
         <v>4174754</v>
@@ -34720,20 +34720,20 @@
       <c r="J5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M5" s="3">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3">
-        <v>1</v>
       </c>
       <c r="P5" s="3">
         <v>1272621</v>
@@ -34770,20 +34770,20 @@
       <c r="J6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="K6" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>20.818200000000001</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M6" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O6" s="3">
-        <v>20.818200000000001</v>
       </c>
       <c r="P6" s="3">
         <v>4174756</v>
@@ -34820,20 +34820,20 @@
       <c r="J7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M7" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N7" s="3">
-        <v>1</v>
-      </c>
-      <c r="O7" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P7" s="3">
         <v>7927534</v>
@@ -34870,20 +34870,20 @@
       <c r="J8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="3">
+        <v>60</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="M8" s="3">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M8" s="3">
-        <v>60</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="O8" s="3">
-        <v>18</v>
       </c>
       <c r="P8" s="3">
         <v>3205740</v>
@@ -34920,20 +34920,20 @@
       <c r="J9" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3">
-        <v>1</v>
       </c>
       <c r="P9" s="3">
         <v>1085353</v>
@@ -34970,20 +34970,20 @@
       <c r="J10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="K10" s="3">
+        <v>60</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="3">
+        <v>30</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M10" s="3">
-        <v>60</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O10" s="3">
-        <v>30</v>
       </c>
       <c r="P10" s="3">
         <v>1271213</v>
@@ -35020,20 +35020,20 @@
       <c r="J11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="K11" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M11" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P11" s="3">
         <v>2812225</v>
@@ -35070,20 +35070,20 @@
       <c r="J12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="K12" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M12" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N12" s="3">
-        <v>2</v>
-      </c>
-      <c r="O12" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P12" s="3">
         <v>4174823</v>
@@ -35120,20 +35120,20 @@
       <c r="J13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="3" t="s">
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M13" s="3">
-        <v>1</v>
-      </c>
-      <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1</v>
       </c>
       <c r="P13" s="3">
         <v>1085547</v>
@@ -35170,20 +35170,20 @@
       <c r="J14" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="K14" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M14" s="3">
+        <v>27.2727</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M14" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N14" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O14" s="3">
-        <v>27.2727</v>
       </c>
       <c r="P14" s="3">
         <v>4006046</v>
@@ -35220,20 +35220,20 @@
       <c r="J15" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L15" s="3">
+        <v>3</v>
+      </c>
+      <c r="M15" s="3">
+        <v>136.36349999999999</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M15" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N15" s="3">
-        <v>3</v>
-      </c>
-      <c r="O15" s="3">
-        <v>136.36349999999999</v>
       </c>
       <c r="P15" s="3">
         <v>7927530</v>
@@ -35270,20 +35270,20 @@
       <c r="J16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M16" s="3">
-        <v>1</v>
-      </c>
-      <c r="N16" s="3">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3">
-        <v>1</v>
       </c>
       <c r="P16" s="3">
         <v>1085363</v>
@@ -35320,20 +35320,20 @@
       <c r="J17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="3" t="s">
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="M17" s="3">
-        <v>1</v>
-      </c>
-      <c r="N17" s="3">
-        <v>1</v>
-      </c>
-      <c r="O17" s="3">
-        <v>1</v>
       </c>
       <c r="P17" s="3">
         <v>30478509</v>
@@ -35370,20 +35370,20 @@
       <c r="J18" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="3" t="s">
+      <c r="K18" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="M18" s="3">
+        <v>68.181799999999996</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M18" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N18" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="O18" s="3">
-        <v>68.181799999999996</v>
       </c>
       <c r="P18" s="3">
         <v>1272043</v>
@@ -35420,20 +35420,20 @@
       <c r="J19" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="3" t="s">
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M19" s="3">
-        <v>1</v>
-      </c>
-      <c r="N19" s="3">
-        <v>1</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1</v>
       </c>
       <c r="P19" s="3">
         <v>1085349</v>
@@ -35470,20 +35470,20 @@
       <c r="J20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="3" t="s">
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M20" s="3">
-        <v>1</v>
-      </c>
-      <c r="N20" s="3">
-        <v>1</v>
-      </c>
-      <c r="O20" s="3">
-        <v>1</v>
       </c>
       <c r="P20" s="3">
         <v>1085368</v>
@@ -35520,20 +35520,20 @@
       <c r="J21" s="3" t="s">
         <v>1155</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3" t="s">
+      <c r="K21" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L21" s="3">
+        <v>9</v>
+      </c>
+      <c r="M21" s="3">
+        <v>936.81809999999996</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M21" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N21" s="3">
-        <v>9</v>
-      </c>
-      <c r="O21" s="3">
-        <v>936.81809999999996</v>
       </c>
       <c r="P21" s="3">
         <v>2837807</v>
@@ -35570,20 +35570,20 @@
       <c r="J22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="3" t="s">
+      <c r="K22" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M22" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N22" s="3">
-        <v>2</v>
-      </c>
-      <c r="O22" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P22" s="3">
         <v>2837813</v>
@@ -35620,20 +35620,20 @@
       <c r="J23" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="3" t="s">
+      <c r="K23" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3">
+        <v>181.81800000000001</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M23" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N23" s="3">
-        <v>4</v>
-      </c>
-      <c r="O23" s="3">
-        <v>181.81800000000001</v>
       </c>
       <c r="P23" s="3">
         <v>3379404</v>
@@ -35670,20 +35670,20 @@
       <c r="J24" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3" t="s">
+      <c r="K24" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>9.0908999999999995</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M24" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N24" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O24" s="3">
-        <v>9.0908999999999995</v>
       </c>
       <c r="P24" s="3">
         <v>1272052</v>
@@ -35720,20 +35720,20 @@
       <c r="J25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3" t="s">
+      <c r="K25" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L25" s="3">
+        <v>2</v>
+      </c>
+      <c r="M25" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O25" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M25" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N25" s="3">
-        <v>2</v>
-      </c>
-      <c r="O25" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P25" s="3">
         <v>1272125</v>
@@ -35770,20 +35770,20 @@
       <c r="J26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="3" t="s">
+      <c r="K26" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L26" s="3">
+        <v>2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O26" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M26" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N26" s="3">
-        <v>2</v>
-      </c>
-      <c r="O26" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P26" s="3">
         <v>4174761</v>
@@ -35820,20 +35820,20 @@
       <c r="J27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="3" t="s">
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="M27" s="3">
-        <v>1</v>
-      </c>
-      <c r="N27" s="3">
-        <v>1</v>
-      </c>
-      <c r="O27" s="3">
-        <v>1</v>
       </c>
       <c r="P27" s="3">
         <v>30478489</v>
@@ -35870,20 +35870,20 @@
       <c r="J28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="3" t="s">
+      <c r="K28" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L28" s="3">
+        <v>2</v>
+      </c>
+      <c r="M28" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M28" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N28" s="3">
-        <v>2</v>
-      </c>
-      <c r="O28" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P28" s="3">
         <v>4174859</v>
@@ -35920,20 +35920,20 @@
       <c r="J29" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="3" t="s">
+      <c r="K29" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L29" s="3">
+        <v>2</v>
+      </c>
+      <c r="M29" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M29" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N29" s="3">
-        <v>2</v>
-      </c>
-      <c r="O29" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P29" s="3">
         <v>3379391</v>
@@ -35970,20 +35970,20 @@
       <c r="J30" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="3" t="s">
+      <c r="K30" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M30" s="3">
+        <v>62.454500000000003</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M30" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N30" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O30" s="3">
-        <v>62.454500000000003</v>
       </c>
       <c r="P30" s="3">
         <v>4174726</v>
@@ -36020,20 +36020,20 @@
       <c r="J31" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="3" t="s">
+      <c r="K31" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L31" s="3">
+        <v>2</v>
+      </c>
+      <c r="M31" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M31" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N31" s="3">
-        <v>2</v>
-      </c>
-      <c r="O31" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P31" s="3">
         <v>2812251</v>
@@ -36070,20 +36070,20 @@
       <c r="J32" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="3" t="s">
+      <c r="K32" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L32" s="3">
+        <v>2</v>
+      </c>
+      <c r="M32" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O32" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M32" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N32" s="3">
-        <v>2</v>
-      </c>
-      <c r="O32" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P32" s="3">
         <v>2812227</v>
@@ -36120,20 +36120,20 @@
       <c r="J33" s="3" t="s">
         <v>1179</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L33" s="3" t="s">
+      <c r="K33" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L33" s="3">
+        <v>2</v>
+      </c>
+      <c r="M33" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O33" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M33" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N33" s="3">
-        <v>2</v>
-      </c>
-      <c r="O33" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P33" s="3">
         <v>2812223</v>
@@ -36170,20 +36170,20 @@
       <c r="J34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="3" t="s">
+      <c r="K34" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="M34" s="3">
+        <v>72.727199999999996</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M34" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N34" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="O34" s="3">
-        <v>72.727199999999996</v>
       </c>
       <c r="P34" s="3">
         <v>4174822</v>
@@ -36220,20 +36220,20 @@
       <c r="J35" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="3" t="s">
+      <c r="K35" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L35" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="M35" s="3">
+        <v>54.545400000000001</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M35" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N35" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="O35" s="3">
-        <v>54.545400000000001</v>
       </c>
       <c r="P35" s="3">
         <v>3422568</v>
@@ -36270,20 +36270,20 @@
       <c r="J36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="3" t="s">
+      <c r="K36" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L36" s="3">
+        <v>2</v>
+      </c>
+      <c r="M36" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M36" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N36" s="3">
-        <v>2</v>
-      </c>
-      <c r="O36" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P36" s="3">
         <v>3379372</v>
@@ -36320,20 +36320,20 @@
       <c r="J37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="3" t="s">
+      <c r="K37" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L37" s="3">
+        <v>1</v>
+      </c>
+      <c r="M37" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O37" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M37" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P37" s="3">
         <v>4174790</v>
@@ -36370,20 +36370,20 @@
       <c r="J38" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="3" t="s">
+      <c r="K38" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L38" s="3">
+        <v>2</v>
+      </c>
+      <c r="M38" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O38" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M38" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N38" s="3">
-        <v>2</v>
-      </c>
-      <c r="O38" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P38" s="3">
         <v>4174773</v>
@@ -36420,20 +36420,20 @@
       <c r="J39" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="3" t="s">
+      <c r="K39" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L39" s="3">
+        <v>2</v>
+      </c>
+      <c r="M39" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O39" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M39" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N39" s="3">
-        <v>2</v>
-      </c>
-      <c r="O39" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P39" s="3">
         <v>2812218</v>
@@ -36470,20 +36470,20 @@
       <c r="J40" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="3" t="s">
+      <c r="K40" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1</v>
+      </c>
+      <c r="M40" s="3">
+        <v>47.727200000000003</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O40" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M40" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N40" s="3">
-        <v>1</v>
-      </c>
-      <c r="O40" s="3">
-        <v>47.727200000000003</v>
       </c>
       <c r="P40" s="3">
         <v>2812219</v>
@@ -36520,20 +36520,20 @@
       <c r="J41" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="3" t="s">
+      <c r="K41" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L41" s="3">
+        <v>1</v>
+      </c>
+      <c r="M41" s="3">
+        <v>47.727200000000003</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O41" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M41" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N41" s="3">
-        <v>1</v>
-      </c>
-      <c r="O41" s="3">
-        <v>47.727200000000003</v>
       </c>
       <c r="P41" s="3">
         <v>2812244</v>
@@ -36570,20 +36570,20 @@
       <c r="J42" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="3" t="s">
+      <c r="K42" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L42" s="3">
+        <v>2</v>
+      </c>
+      <c r="M42" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O42" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M42" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N42" s="3">
-        <v>2</v>
-      </c>
-      <c r="O42" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P42" s="3">
         <v>4174864</v>
@@ -36620,20 +36620,20 @@
       <c r="J43" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="3" t="s">
+      <c r="K43" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L43" s="3">
+        <v>6</v>
+      </c>
+      <c r="M43" s="3">
+        <v>272.72699999999998</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O43" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M43" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N43" s="3">
-        <v>6</v>
-      </c>
-      <c r="O43" s="3">
-        <v>272.72699999999998</v>
       </c>
       <c r="P43" s="3">
         <v>2812224</v>
@@ -36670,20 +36670,20 @@
       <c r="J44" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="3" t="s">
+      <c r="K44" s="3">
+        <v>1</v>
+      </c>
+      <c r="L44" s="3">
+        <v>10</v>
+      </c>
+      <c r="M44" s="3">
+        <v>10</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M44" s="3">
-        <v>1</v>
-      </c>
-      <c r="N44" s="3">
-        <v>10</v>
-      </c>
-      <c r="O44" s="3">
-        <v>10</v>
       </c>
       <c r="P44" s="3">
         <v>1272053</v>
@@ -36720,20 +36720,20 @@
       <c r="J45" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="3" t="s">
+      <c r="K45" s="3">
+        <v>1</v>
+      </c>
+      <c r="L45" s="3">
+        <v>1</v>
+      </c>
+      <c r="M45" s="3">
+        <v>1</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O45" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M45" s="3">
-        <v>1</v>
-      </c>
-      <c r="N45" s="3">
-        <v>1</v>
-      </c>
-      <c r="O45" s="3">
-        <v>1</v>
       </c>
       <c r="P45" s="3">
         <v>1085543</v>
@@ -36770,20 +36770,20 @@
       <c r="J46" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="3" t="s">
+      <c r="K46" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L46" s="3">
+        <v>1</v>
+      </c>
+      <c r="M46" s="3">
+        <v>47.727200000000003</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O46" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M46" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N46" s="3">
-        <v>1</v>
-      </c>
-      <c r="O46" s="3">
-        <v>47.727200000000003</v>
       </c>
       <c r="P46" s="3">
         <v>2812315</v>
@@ -36820,20 +36820,20 @@
       <c r="J47" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="3" t="s">
+      <c r="K47" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L47" s="3">
+        <v>1</v>
+      </c>
+      <c r="M47" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O47" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M47" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N47" s="3">
-        <v>1</v>
-      </c>
-      <c r="O47" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P47" s="3">
         <v>4174835</v>
@@ -36870,20 +36870,20 @@
       <c r="J48" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="3" t="s">
+      <c r="K48" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L48" s="3">
+        <v>3</v>
+      </c>
+      <c r="M48" s="3">
+        <v>136.36349999999999</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O48" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M48" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N48" s="3">
-        <v>3</v>
-      </c>
-      <c r="O48" s="3">
-        <v>136.36349999999999</v>
       </c>
       <c r="P48" s="3">
         <v>2812214</v>
@@ -36920,20 +36920,20 @@
       <c r="J49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L49" s="3">
+        <v>6</v>
+      </c>
+      <c r="M49" s="3">
+        <v>624.54539999999997</v>
+      </c>
+      <c r="N49" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L49" s="3" t="s">
+      <c r="O49" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M49" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N49" s="3">
-        <v>6</v>
-      </c>
-      <c r="O49" s="3">
-        <v>624.54539999999997</v>
       </c>
       <c r="P49" s="3">
         <v>7927648</v>
@@ -36970,20 +36970,20 @@
       <c r="J50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="3" t="s">
+      <c r="K50" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L50" s="3">
+        <v>6</v>
+      </c>
+      <c r="M50" s="3">
+        <v>272.72699999999998</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O50" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M50" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N50" s="3">
-        <v>6</v>
-      </c>
-      <c r="O50" s="3">
-        <v>272.72699999999998</v>
       </c>
       <c r="P50" s="3">
         <v>2812321</v>
@@ -37020,20 +37020,20 @@
       <c r="J51" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="3" t="s">
+      <c r="K51" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L51" s="3">
+        <v>4</v>
+      </c>
+      <c r="M51" s="3">
+        <v>416.36360000000002</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O51" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M51" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N51" s="3">
-        <v>4</v>
-      </c>
-      <c r="O51" s="3">
-        <v>416.36360000000002</v>
       </c>
       <c r="P51" s="3">
         <v>2837811</v>
@@ -37070,20 +37070,20 @@
       <c r="J52" s="3" t="s">
         <v>1210</v>
       </c>
-      <c r="K52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="3" t="s">
+      <c r="K52" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L52" s="3">
+        <v>2</v>
+      </c>
+      <c r="M52" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O52" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M52" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N52" s="3">
-        <v>2</v>
-      </c>
-      <c r="O52" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P52" s="3">
         <v>4174721</v>
@@ -37120,20 +37120,20 @@
       <c r="J53" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L53" s="3">
+        <v>4</v>
+      </c>
+      <c r="M53" s="3">
+        <v>181.81800000000001</v>
+      </c>
+      <c r="N53" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L53" s="3" t="s">
+      <c r="O53" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M53" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N53" s="3">
-        <v>4</v>
-      </c>
-      <c r="O53" s="3">
-        <v>181.81800000000001</v>
       </c>
       <c r="P53" s="3">
         <v>7927577</v>
@@ -37170,20 +37170,20 @@
       <c r="J54" s="3" t="s">
         <v>1214</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L54" s="3" t="s">
+      <c r="K54" s="3">
+        <v>1</v>
+      </c>
+      <c r="L54" s="3">
+        <v>20</v>
+      </c>
+      <c r="M54" s="3">
+        <v>20</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O54" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M54" s="3">
-        <v>1</v>
-      </c>
-      <c r="N54" s="3">
-        <v>20</v>
-      </c>
-      <c r="O54" s="3">
-        <v>20</v>
       </c>
       <c r="P54" s="3">
         <v>4174811</v>
@@ -37220,20 +37220,20 @@
       <c r="J55" s="3" t="s">
         <v>1217</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" s="3" t="s">
+      <c r="K55" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L55" s="3">
+        <v>2</v>
+      </c>
+      <c r="M55" s="3">
+        <v>90.9</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O55" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M55" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N55" s="3">
-        <v>2</v>
-      </c>
-      <c r="O55" s="3">
-        <v>90.9</v>
       </c>
       <c r="P55" s="3">
         <v>2812228</v>
@@ -37270,20 +37270,20 @@
       <c r="J56" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="3" t="s">
+      <c r="K56" s="3">
+        <v>1</v>
+      </c>
+      <c r="L56" s="3">
+        <v>1</v>
+      </c>
+      <c r="M56" s="3">
+        <v>1</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O56" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M56" s="3">
-        <v>1</v>
-      </c>
-      <c r="N56" s="3">
-        <v>1</v>
-      </c>
-      <c r="O56" s="3">
-        <v>1</v>
       </c>
       <c r="P56" s="3">
         <v>1005889</v>
@@ -37320,20 +37320,20 @@
       <c r="J57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K57" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" s="3" t="s">
+      <c r="K57" s="3">
+        <v>1</v>
+      </c>
+      <c r="L57" s="3">
+        <v>1</v>
+      </c>
+      <c r="M57" s="3">
+        <v>1</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O57" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M57" s="3">
-        <v>1</v>
-      </c>
-      <c r="N57" s="3">
-        <v>1</v>
-      </c>
-      <c r="O57" s="3">
-        <v>1</v>
       </c>
       <c r="P57" s="3">
         <v>1005892</v>
@@ -37370,20 +37370,20 @@
       <c r="J58" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="K58" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L58" s="3" t="s">
+      <c r="K58" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L58" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="M58" s="3">
+        <v>72.727199999999996</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O58" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M58" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N58" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="O58" s="3">
-        <v>72.727199999999996</v>
       </c>
       <c r="P58" s="3">
         <v>1272020</v>
@@ -37420,20 +37420,20 @@
       <c r="J59" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="K59" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L59" s="3" t="s">
+      <c r="K59" s="3">
+        <v>1</v>
+      </c>
+      <c r="L59" s="3">
+        <v>50</v>
+      </c>
+      <c r="M59" s="3">
+        <v>50</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O59" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M59" s="3">
-        <v>1</v>
-      </c>
-      <c r="N59" s="3">
-        <v>50</v>
-      </c>
-      <c r="O59" s="3">
-        <v>50</v>
       </c>
       <c r="P59" s="3">
         <v>4174783</v>
@@ -37470,20 +37470,20 @@
       <c r="J60" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K60" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L60" s="3" t="s">
+      <c r="K60" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M60" s="3">
+        <v>22.7273</v>
+      </c>
+      <c r="N60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O60" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M60" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N60" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O60" s="3">
-        <v>22.7273</v>
       </c>
       <c r="P60" s="3">
         <v>1271592</v>
@@ -37520,20 +37520,20 @@
       <c r="J61" s="3" t="s">
         <v>1227</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K61" s="3">
+        <v>83.33</v>
+      </c>
+      <c r="L61" s="3">
+        <v>100</v>
+      </c>
+      <c r="M61" s="3">
+        <v>8333.33</v>
+      </c>
+      <c r="N61" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="O61" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M61" s="3">
-        <v>83.33</v>
-      </c>
-      <c r="N61" s="3">
-        <v>100</v>
-      </c>
-      <c r="O61" s="3">
-        <v>8333.33</v>
       </c>
       <c r="P61" s="3">
         <v>7927627</v>
@@ -37570,20 +37570,20 @@
       <c r="J62" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K62" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L62" s="3" t="s">
+      <c r="K62" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L62" s="3">
+        <v>1</v>
+      </c>
+      <c r="M62" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O62" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M62" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N62" s="3">
-        <v>1</v>
-      </c>
-      <c r="O62" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P62" s="3">
         <v>4174815</v>
@@ -37620,20 +37620,20 @@
       <c r="J63" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="K63" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L63" s="3" t="s">
+      <c r="K63" s="3">
+        <v>1</v>
+      </c>
+      <c r="L63" s="3">
+        <v>12</v>
+      </c>
+      <c r="M63" s="3">
+        <v>12</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O63" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M63" s="3">
-        <v>1</v>
-      </c>
-      <c r="N63" s="3">
-        <v>12</v>
-      </c>
-      <c r="O63" s="3">
-        <v>12</v>
       </c>
       <c r="P63" s="3">
         <v>4174741</v>
@@ -37670,20 +37670,20 @@
       <c r="J64" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K64" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L64" s="3" t="s">
+      <c r="K64" s="3">
+        <v>1</v>
+      </c>
+      <c r="L64" s="3">
+        <v>20</v>
+      </c>
+      <c r="M64" s="3">
+        <v>20</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O64" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M64" s="3">
-        <v>1</v>
-      </c>
-      <c r="N64" s="3">
-        <v>20</v>
-      </c>
-      <c r="O64" s="3">
-        <v>20</v>
       </c>
       <c r="P64" s="3">
         <v>2812215</v>
@@ -37720,20 +37720,20 @@
       <c r="J65" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K65" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L65" s="3" t="s">
+      <c r="K65" s="3">
+        <v>1</v>
+      </c>
+      <c r="L65" s="3">
+        <v>1</v>
+      </c>
+      <c r="M65" s="3">
+        <v>1</v>
+      </c>
+      <c r="N65" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O65" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M65" s="3">
-        <v>1</v>
-      </c>
-      <c r="N65" s="3">
-        <v>1</v>
-      </c>
-      <c r="O65" s="3">
-        <v>1</v>
       </c>
       <c r="P65" s="3">
         <v>1085528</v>
@@ -37770,20 +37770,20 @@
       <c r="J66" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="K66" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66" s="3" t="s">
+      <c r="K66" s="3">
+        <v>1</v>
+      </c>
+      <c r="L66" s="3">
+        <v>50</v>
+      </c>
+      <c r="M66" s="3">
+        <v>50</v>
+      </c>
+      <c r="N66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O66" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M66" s="3">
-        <v>1</v>
-      </c>
-      <c r="N66" s="3">
-        <v>50</v>
-      </c>
-      <c r="O66" s="3">
-        <v>50</v>
       </c>
       <c r="P66" s="3">
         <v>2812320</v>
@@ -37820,20 +37820,20 @@
       <c r="J67" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="K67" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L67" s="3" t="s">
+      <c r="K67" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M67" s="3">
+        <v>52.045499999999997</v>
+      </c>
+      <c r="N67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O67" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M67" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N67" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O67" s="3">
-        <v>52.045499999999997</v>
       </c>
       <c r="P67" s="3">
         <v>2812222</v>
@@ -37870,20 +37870,20 @@
       <c r="J68" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="K68" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L68" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="M68" s="3">
+        <v>333.09089999999998</v>
+      </c>
+      <c r="N68" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="O68" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M68" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N68" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="O68" s="3">
-        <v>333.09089999999998</v>
       </c>
       <c r="P68" s="3">
         <v>7927547</v>
@@ -37920,20 +37920,20 @@
       <c r="J69" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="K69" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L69" s="3" t="s">
+      <c r="K69" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L69" s="3">
+        <v>2</v>
+      </c>
+      <c r="M69" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N69" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O69" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M69" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N69" s="3">
-        <v>2</v>
-      </c>
-      <c r="O69" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P69" s="3">
         <v>4174863</v>
@@ -37970,20 +37970,20 @@
       <c r="J70" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K70" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L70" s="3" t="s">
+      <c r="K70" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M70" s="3">
+        <v>20.818200000000001</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O70" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M70" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N70" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O70" s="3">
-        <v>20.818200000000001</v>
       </c>
       <c r="P70" s="3">
         <v>2812229</v>
@@ -38020,20 +38020,20 @@
       <c r="J71" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K71" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L71" s="3" t="s">
+      <c r="K71" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L71" s="3">
+        <v>2</v>
+      </c>
+      <c r="M71" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N71" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O71" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M71" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N71" s="3">
-        <v>2</v>
-      </c>
-      <c r="O71" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P71" s="3">
         <v>4174748</v>
@@ -38070,20 +38070,20 @@
       <c r="J72" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="K72" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L72" s="3" t="s">
+      <c r="K72" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L72" s="3">
+        <v>2</v>
+      </c>
+      <c r="M72" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O72" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M72" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N72" s="3">
-        <v>2</v>
-      </c>
-      <c r="O72" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P72" s="3">
         <v>2812306</v>
@@ -38120,20 +38120,20 @@
       <c r="J73" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K73" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L73" s="3" t="s">
+      <c r="K73" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L73" s="3">
+        <v>2</v>
+      </c>
+      <c r="M73" s="3">
+        <v>90.909000000000006</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O73" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M73" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N73" s="3">
-        <v>2</v>
-      </c>
-      <c r="O73" s="3">
-        <v>90.909000000000006</v>
       </c>
       <c r="P73" s="3">
         <v>1272046</v>
@@ -38170,20 +38170,20 @@
       <c r="J74" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="K74" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L74" s="3" t="s">
+      <c r="K74" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L74" s="3">
+        <v>2</v>
+      </c>
+      <c r="M74" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O74" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M74" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N74" s="3">
-        <v>2</v>
-      </c>
-      <c r="O74" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P74" s="3">
         <v>2837812</v>
@@ -38220,20 +38220,20 @@
       <c r="J75" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K75" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L75" s="3" t="s">
+      <c r="K75" s="3">
+        <v>1</v>
+      </c>
+      <c r="L75" s="3">
+        <v>20</v>
+      </c>
+      <c r="M75" s="3">
+        <v>20</v>
+      </c>
+      <c r="N75" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O75" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M75" s="3">
-        <v>1</v>
-      </c>
-      <c r="N75" s="3">
-        <v>20</v>
-      </c>
-      <c r="O75" s="3">
-        <v>20</v>
       </c>
       <c r="P75" s="3">
         <v>4174753</v>
@@ -38270,20 +38270,20 @@
       <c r="J76" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K76" s="3" t="s">
+      <c r="K76" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L76" s="3">
+        <v>2</v>
+      </c>
+      <c r="M76" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N76" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L76" s="3" t="s">
+      <c r="O76" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M76" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N76" s="3">
-        <v>2</v>
-      </c>
-      <c r="O76" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P76" s="3">
         <v>7927575</v>
@@ -38320,20 +38320,20 @@
       <c r="J77" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K77" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L77" s="3" t="s">
+      <c r="K77" s="3">
+        <v>1</v>
+      </c>
+      <c r="L77" s="3">
+        <v>40</v>
+      </c>
+      <c r="M77" s="3">
+        <v>40</v>
+      </c>
+      <c r="N77" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O77" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M77" s="3">
-        <v>1</v>
-      </c>
-      <c r="N77" s="3">
-        <v>40</v>
-      </c>
-      <c r="O77" s="3">
-        <v>40</v>
       </c>
       <c r="P77" s="3">
         <v>1271571</v>
@@ -38370,20 +38370,20 @@
       <c r="J78" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K78" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L78" s="3" t="s">
+      <c r="K78" s="3">
+        <v>1</v>
+      </c>
+      <c r="L78" s="3">
+        <v>1</v>
+      </c>
+      <c r="M78" s="3">
+        <v>1</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O78" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M78" s="3">
-        <v>1</v>
-      </c>
-      <c r="N78" s="3">
-        <v>1</v>
-      </c>
-      <c r="O78" s="3">
-        <v>1</v>
       </c>
       <c r="P78" s="3">
         <v>1085529</v>
@@ -38420,20 +38420,20 @@
       <c r="J79" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K79" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L79" s="3" t="s">
+      <c r="K79" s="3">
+        <v>1</v>
+      </c>
+      <c r="L79" s="3">
+        <v>50</v>
+      </c>
+      <c r="M79" s="3">
+        <v>50</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O79" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M79" s="3">
-        <v>1</v>
-      </c>
-      <c r="N79" s="3">
-        <v>50</v>
-      </c>
-      <c r="O79" s="3">
-        <v>50</v>
       </c>
       <c r="P79" s="3">
         <v>4006040</v>
@@ -38470,20 +38470,20 @@
       <c r="J80" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K80" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L80" s="3" t="s">
+      <c r="K80" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L80" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M80" s="3">
+        <v>9.0908999999999995</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O80" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M80" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N80" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O80" s="3">
-        <v>9.0908999999999995</v>
       </c>
       <c r="P80" s="3">
         <v>3422569</v>
@@ -38520,20 +38520,20 @@
       <c r="J81" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K81" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L81" s="3" t="s">
+      <c r="K81" s="3">
+        <v>1</v>
+      </c>
+      <c r="L81" s="3">
+        <v>12</v>
+      </c>
+      <c r="M81" s="3">
+        <v>12</v>
+      </c>
+      <c r="N81" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O81" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M81" s="3">
-        <v>1</v>
-      </c>
-      <c r="N81" s="3">
-        <v>12</v>
-      </c>
-      <c r="O81" s="3">
-        <v>12</v>
       </c>
       <c r="P81" s="3">
         <v>3422544</v>
@@ -38570,20 +38570,20 @@
       <c r="J82" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="K82" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L82" s="3" t="s">
+      <c r="K82" s="3">
+        <v>1</v>
+      </c>
+      <c r="L82" s="3">
+        <v>20</v>
+      </c>
+      <c r="M82" s="3">
+        <v>20</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O82" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M82" s="3">
-        <v>1</v>
-      </c>
-      <c r="N82" s="3">
-        <v>20</v>
-      </c>
-      <c r="O82" s="3">
-        <v>20</v>
       </c>
       <c r="P82" s="3">
         <v>4174853</v>
@@ -38620,20 +38620,20 @@
       <c r="J83" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K83" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L83" s="3" t="s">
+      <c r="K83" s="3">
+        <v>60</v>
+      </c>
+      <c r="L83" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M83" s="3">
+        <v>36</v>
+      </c>
+      <c r="N83" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O83" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M83" s="3">
-        <v>60</v>
-      </c>
-      <c r="N83" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O83" s="3">
-        <v>36</v>
       </c>
       <c r="P83" s="3">
         <v>4174765</v>
@@ -38670,20 +38670,20 @@
       <c r="J84" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K84" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L84" s="3" t="s">
+      <c r="K84" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L84" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M84" s="3">
+        <v>10.41</v>
+      </c>
+      <c r="N84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O84" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M84" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N84" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="O84" s="3">
-        <v>10.41</v>
       </c>
       <c r="P84" s="3">
         <v>3379386</v>
@@ -38720,20 +38720,20 @@
       <c r="J85" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K85" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L85" s="3" t="s">
+      <c r="K85" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L85" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M85" s="3">
+        <v>20.818200000000001</v>
+      </c>
+      <c r="N85" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O85" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M85" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N85" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="O85" s="3">
-        <v>20.818200000000001</v>
       </c>
       <c r="P85" s="3">
         <v>3422523</v>
@@ -38770,20 +38770,20 @@
       <c r="J86" s="3" t="s">
         <v>1266</v>
       </c>
-      <c r="K86" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L86" s="3" t="s">
+      <c r="K86" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L86" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="M86" s="3">
+        <v>54.545400000000001</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O86" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M86" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N86" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="O86" s="3">
-        <v>54.545400000000001</v>
       </c>
       <c r="P86" s="3">
         <v>2812220</v>
@@ -38820,20 +38820,20 @@
       <c r="J87" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="K87" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L87" s="3" t="s">
+      <c r="K87" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L87" s="3">
+        <v>2</v>
+      </c>
+      <c r="M87" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N87" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O87" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M87" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N87" s="3">
-        <v>2</v>
-      </c>
-      <c r="O87" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P87" s="3">
         <v>2812221</v>
@@ -38870,20 +38870,20 @@
       <c r="J88" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K88" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L88" s="3" t="s">
+      <c r="K88" s="3">
+        <v>104.09</v>
+      </c>
+      <c r="L88" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M88" s="3">
+        <v>62.454500000000003</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O88" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M88" s="3">
-        <v>104.09</v>
-      </c>
-      <c r="N88" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O88" s="3">
-        <v>62.454500000000003</v>
       </c>
       <c r="P88" s="3">
         <v>2812211</v>
@@ -38920,20 +38920,20 @@
       <c r="J89" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K89" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L89" s="3" t="s">
+      <c r="K89" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L89" s="3">
+        <v>1</v>
+      </c>
+      <c r="M89" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O89" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M89" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N89" s="3">
-        <v>1</v>
-      </c>
-      <c r="O89" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P89" s="3">
         <v>3379387</v>
@@ -38970,20 +38970,20 @@
       <c r="J90" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="K90" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L90" s="3" t="s">
+      <c r="K90" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L90" s="3">
+        <v>1</v>
+      </c>
+      <c r="M90" s="3">
+        <v>45.454500000000003</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O90" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M90" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N90" s="3">
-        <v>1</v>
-      </c>
-      <c r="O90" s="3">
-        <v>45.454500000000003</v>
       </c>
       <c r="P90" s="3">
         <v>3422582</v>
@@ -39020,20 +39020,20 @@
       <c r="J91" s="3" t="s">
         <v>1275</v>
       </c>
-      <c r="K91" s="3" t="s">
+      <c r="K91" s="3">
+        <v>45.45</v>
+      </c>
+      <c r="L91" s="3">
+        <v>3</v>
+      </c>
+      <c r="M91" s="3">
+        <v>136.36349999999999</v>
+      </c>
+      <c r="N91" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L91" s="3" t="s">
+      <c r="O91" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="M91" s="3">
-        <v>45.45</v>
-      </c>
-      <c r="N91" s="3">
-        <v>3</v>
-      </c>
-      <c r="O91" s="3">
-        <v>136.36349999999999</v>
       </c>
       <c r="P91" s="3">
         <v>7927573</v>
@@ -39070,20 +39070,20 @@
       <c r="J92" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="K92" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L92" s="3" t="s">
+      <c r="K92" s="3">
+        <v>47.73</v>
+      </c>
+      <c r="L92" s="3">
+        <v>2</v>
+      </c>
+      <c r="M92" s="3">
+        <v>95.454400000000007</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O92" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M92" s="3">
-        <v>47.73</v>
-      </c>
-      <c r="N92" s="3">
-        <v>2</v>
-      </c>
-      <c r="O92" s="3">
-        <v>95.454400000000007</v>
       </c>
       <c r="P92" s="3">
         <v>2812313</v>
@@ -39120,20 +39120,20 @@
       <c r="J93" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="K93" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L93" s="3" t="s">
+      <c r="K93" s="3">
+        <v>1</v>
+      </c>
+      <c r="L93" s="3">
+        <v>10</v>
+      </c>
+      <c r="M93" s="3">
+        <v>10</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O93" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="M93" s="3">
-        <v>1</v>
-      </c>
-      <c r="N93" s="3">
-        <v>10</v>
-      </c>
-      <c r="O93" s="3">
-        <v>10</v>
       </c>
       <c r="P93" s="3">
         <v>4174867</v>
@@ -39170,27 +39170,27 @@
       <c r="J94" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K94" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L94" s="3" t="s">
+      <c r="K94" s="3">
+        <v>1</v>
+      </c>
+      <c r="L94" s="3">
+        <v>1</v>
+      </c>
+      <c r="M94" s="3">
+        <v>1</v>
+      </c>
+      <c r="N94" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O94" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="M94" s="3">
-        <v>1</v>
-      </c>
-      <c r="N94" s="3">
-        <v>1</v>
-      </c>
-      <c r="O94" s="3">
-        <v>1</v>
       </c>
       <c r="P94" s="3">
         <v>30478478</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:EQ94">
+  <autoFilter ref="A1:EN94">
     <sortState ref="A2:EQ94">
       <sortCondition ref="D1:D94"/>
     </sortState>
@@ -39203,7 +39203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -44685,7 +44685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -44737,10 +44737,10 @@
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="14" t="s">
         <v>521</v>
       </c>
@@ -44757,16 +44757,16 @@
         <v>20</v>
       </c>
       <c r="I2" s="8">
-        <f>+G2*H2</f>
+        <f t="shared" ref="I2:I17" si="0">+G2*H2</f>
         <v>909.09</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="17" t="s">
+      <c r="J2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="16">
         <v>2812297</v>
       </c>
     </row>
@@ -44774,10 +44774,10 @@
       <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="14" t="s">
         <v>521</v>
       </c>
@@ -44794,16 +44794,16 @@
         <v>20</v>
       </c>
       <c r="I3" s="8">
-        <f>+G3*H3</f>
+        <f t="shared" si="0"/>
         <v>909.09</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="17" t="s">
+      <c r="J3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="16">
         <v>2812276</v>
       </c>
     </row>
@@ -44811,17 +44811,17 @@
       <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="17" t="s">
         <v>1473</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>1474</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>1284</v>
       </c>
       <c r="G4" s="7">
@@ -44831,16 +44831,16 @@
         <v>36</v>
       </c>
       <c r="I4" s="8">
-        <f>+G4*H4</f>
+        <f t="shared" si="0"/>
         <v>1636.3620000000001</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="17" t="s">
+      <c r="J4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="18">
         <v>2828049</v>
       </c>
     </row>
@@ -44848,17 +44848,17 @@
       <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="17" t="s">
         <v>1475</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>1476</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>1284</v>
       </c>
       <c r="G5" s="7">
@@ -44868,16 +44868,16 @@
         <v>5</v>
       </c>
       <c r="I5" s="8">
-        <f>+G5*H5</f>
+        <f t="shared" si="0"/>
         <v>520.45450000000005</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
         <v>1477</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="16">
         <v>6677067</v>
       </c>
     </row>
@@ -44885,17 +44885,17 @@
       <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="19" t="s">
         <v>1478</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>1479</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>1284</v>
       </c>
       <c r="G6" s="7">
@@ -44905,16 +44905,16 @@
         <v>6</v>
       </c>
       <c r="I6" s="8">
-        <f>+G6*H6</f>
+        <f t="shared" si="0"/>
         <v>272.72700000000003</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="19">
         <v>7927616</v>
       </c>
     </row>
@@ -44922,14 +44922,14 @@
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="17" t="s">
         <v>1480</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>1481</v>
       </c>
       <c r="F7" s="14" t="s">
@@ -44942,16 +44942,16 @@
         <v>6</v>
       </c>
       <c r="I7" s="10">
-        <f>+G7*H7</f>
+        <f t="shared" si="0"/>
         <v>272.72700000000003</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="17" t="s">
+      <c r="J7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>4174840</v>
       </c>
     </row>
@@ -44959,14 +44959,14 @@
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>1482</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -44979,16 +44979,16 @@
         <v>5</v>
       </c>
       <c r="I8" s="8">
-        <f>+G8*H8</f>
+        <f t="shared" si="0"/>
         <v>227.27250000000001</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="17" t="s">
+      <c r="J8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>7245463</v>
       </c>
     </row>
@@ -44996,14 +44996,14 @@
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="18" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>1483</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -45016,16 +45016,16 @@
         <v>24</v>
       </c>
       <c r="I9" s="8">
-        <f>+G9*H9</f>
+        <f t="shared" si="0"/>
         <v>1145.4528</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <v>7927622</v>
       </c>
     </row>
@@ -45033,14 +45033,14 @@
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>1484</v>
       </c>
       <c r="F10" s="14" t="s">
@@ -45053,16 +45053,16 @@
         <v>10</v>
       </c>
       <c r="I10" s="8">
-        <f>+G10*H10</f>
+        <f t="shared" si="0"/>
         <v>454.54500000000002</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>2811841</v>
       </c>
     </row>
@@ -45070,14 +45070,14 @@
       <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="17" t="s">
         <v>1485</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>1486</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -45090,16 +45090,16 @@
         <v>20</v>
       </c>
       <c r="I11" s="8">
-        <f>+G11*H11</f>
+        <f t="shared" si="0"/>
         <v>954.5440000000001</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="20">
         <v>6677061</v>
       </c>
     </row>
@@ -45107,14 +45107,14 @@
       <c r="A12" s="14">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="17" t="s">
         <v>1487</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>1488</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -45127,16 +45127,16 @@
         <v>4</v>
       </c>
       <c r="I12" s="10">
-        <f>+G12*H12</f>
+        <f t="shared" si="0"/>
         <v>181.81800000000001</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="16">
         <v>6677063</v>
       </c>
     </row>
@@ -45144,14 +45144,14 @@
       <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="17" t="s">
         <v>1489</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>1490</v>
       </c>
       <c r="F13" s="14" t="s">
@@ -45164,16 +45164,16 @@
         <v>16</v>
       </c>
       <c r="I13" s="8">
-        <f>+G13*H13</f>
+        <f t="shared" si="0"/>
         <v>727.27200000000005</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="17" t="s">
+      <c r="J13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <v>2811836</v>
       </c>
     </row>
@@ -45181,14 +45181,14 @@
       <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="17" t="s">
         <v>1491</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="F14" s="14" t="s">
@@ -45201,16 +45201,16 @@
         <v>12</v>
       </c>
       <c r="I14" s="10">
-        <f>+G14*H14</f>
+        <f t="shared" si="0"/>
         <v>572.72640000000001</v>
       </c>
-      <c r="J14" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="17" t="s">
+      <c r="J14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="16">
         <v>4167699</v>
       </c>
     </row>
@@ -45218,14 +45218,14 @@
       <c r="A15" s="14">
         <v>14</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="17" t="s">
         <v>1493</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>1284</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -45238,16 +45238,16 @@
         <v>14</v>
       </c>
       <c r="I15" s="10">
-        <f>+G15*H15</f>
+        <f t="shared" si="0"/>
         <v>636.36300000000006</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="16">
         <v>7927618</v>
       </c>
     </row>
@@ -45255,14 +45255,14 @@
       <c r="A16" s="14">
         <v>15</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="17" t="s">
         <v>1494</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>1495</v>
       </c>
       <c r="F16" s="14" t="s">
@@ -45275,16 +45275,16 @@
         <v>20</v>
       </c>
       <c r="I16" s="10">
-        <f>+G16*H16</f>
+        <f t="shared" si="0"/>
         <v>909.09</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="17" t="s">
+      <c r="J16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="16">
         <v>3422596</v>
       </c>
     </row>
@@ -45292,14 +45292,14 @@
       <c r="A17" s="14">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="21" t="s">
         <v>1469</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="17" t="s">
         <v>1496</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>1497</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -45312,21 +45312,27 @@
         <v>15</v>
       </c>
       <c r="I17" s="10">
-        <f>+G17*H17</f>
+        <f t="shared" si="0"/>
         <v>681.8175</v>
       </c>
-      <c r="J17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="17" t="s">
+      <c r="J17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="16">
         <v>9644301</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -45337,12 +45343,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>